<commit_message>
updated suite files for all the reports module with logins for each report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCICA/CICA_Login.xlsx
+++ b/src/test/resources/testdataCICA/CICA_Login.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E2891A-3D8B-435F-92B0-0CF764ED6B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BBD06-C512-451D-A107-959182691790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1776" yWindow="576" windowWidth="15576" windowHeight="11664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed the login to level 8 for other modules suite
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCICA/CICA_Login.xlsx
+++ b/src/test/resources/testdataCICA/CICA_Login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40BBD06-C512-451D-A107-959182691790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FABFDF8-92C6-43F2-8BEE-96042D848D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1776" yWindow="576" windowWidth="15576" windowHeight="11664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added suites for dashboard,customer,policy payment modules
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCICA/CICA_Login.xlsx
+++ b/src/test/resources/testdataCICA/CICA_Login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FABFDF8-92C6-43F2-8BEE-96042D848D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F37189-D17D-4C7C-B331-EEEAA8B2D1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1776" yWindow="576" windowWidth="15576" windowHeight="11664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
changed the login credentails
</commit_message>
<xml_diff>
--- a/src/test/resources/testdataCICA/CICA_Login.xlsx
+++ b/src/test/resources/testdataCICA/CICA_Login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F37189-D17D-4C7C-B331-EEEAA8B2D1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8AD685-5347-415A-81DE-F3171ADC1941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1776" yWindow="576" windowWidth="15576" windowHeight="11664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>